<commit_message>
Observations and graphs code modified.
</commit_message>
<xml_diff>
--- a/observations.xlsx
+++ b/observations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anush\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anush\Downloads\LendingClubCaseStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9127B7A4-1EBC-49C6-A17A-0867134424FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D002AC0-6C82-4DF4-85EA-B78746FCD4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCCAC114-ED45-4CA1-8F45-CD351BD65DBC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
   <si>
     <t>Graph</t>
   </si>
@@ -185,6 +185,64 @@
   </si>
   <si>
     <t>18k - 20k loan amount have more charged off in F grade</t>
+  </si>
+  <si>
+    <t>annual_inc_cat, loan_status</t>
+  </si>
+  <si>
+    <t>More Charged off in 30k to 60k range</t>
+  </si>
+  <si>
+    <t>purpose, loan_status,annual_inc</t>
+  </si>
+  <si>
+    <t>Annual income with 50k to 60k with purpose home improvement have more charged off</t>
+  </si>
+  <si>
+    <t>int_rate_cat,annual_inc,loan_status</t>
+  </si>
+  <si>
+    <t>Interest rate 20 to 25 percentage  with annual income 60000+ have more charged off</t>
+  </si>
+  <si>
+    <t>purpose, loan_status, int_rate</t>
+  </si>
+  <si>
+    <t>Loan taken for house purpose has more charged off</t>
+  </si>
+  <si>
+    <t>int_rate, grade, loan_status</t>
+  </si>
+  <si>
+    <t>Interest high with grade G has more defaulters</t>
+  </si>
+  <si>
+    <t>home_ownership, loan_status,annual_inc</t>
+  </si>
+  <si>
+    <t>Mortgage home ownership with 60000 annual income have more charged off</t>
+  </si>
+  <si>
+    <t>annual_inc_cat, loan_status, int_rate</t>
+  </si>
+  <si>
+    <t>Annual income with 90k-120k having high interest rate have more charged off</t>
+  </si>
+  <si>
+    <t>issue_year, loan_status</t>
+  </si>
+  <si>
+    <t>In 2011 Charged off loans are more as per the above graph</t>
+  </si>
+  <si>
+    <t>Correlation Matrix between columns</t>
+  </si>
+  <si>
+    <t>positive correlation at revol_util and int_rate
+positive correlation at loan amount approved ratio and year issued</t>
+  </si>
+  <si>
+    <t>Correlation Matrix</t>
   </si>
 </sst>
 </file>
@@ -278,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -294,7 +352,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8611E034-0D86-42A3-9E81-613ADD71465A}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,7 +724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -678,7 +735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -833,35 +890,35 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -872,19 +929,110 @@
       <c r="B24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:B5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>